<commit_message>
new cells in lda
</commit_message>
<xml_diff>
--- a/latent dirichlet allocation topics.xlsx
+++ b/latent dirichlet allocation topics.xlsx
@@ -34,16 +34,16 @@
     <t>pay,month,job,year,money,payment,time,work,make,credit,go,one,people,could,help,like,college,even,back,going</t>
   </si>
   <si>
-    <t>payment,interest,pay,amount,rate,month,year,paid,paying,balance,principal,time,made,one,monthly,making,applied,owe,make,money</t>
-  </si>
-  <si>
-    <t>forbearance,told,received,deferment,form,letter,month,said,could,application,back,called,sent,repayment,time,stating,paperwork,rep,year,college</t>
-  </si>
-  <si>
-    <t>account,payment,customer,credit,service,check,sent,called,received,told,information,representative,letter,bank,delinquent,issue,report,back,could,day</t>
-  </si>
-  <si>
-    <t>call,phone,day,told,time,said,called,number,calling,asked,payment,even,know,back,one,never,got,person,stop,someone</t>
+    <t>payment,interest,pay,amount,rate,year,month,paid,paying,balance,principal,time,made,monthly,one,making,applied,owe,make,money</t>
+  </si>
+  <si>
+    <t>forbearance,told,received,deferment,form,letter,month,said,could,application,back,sent,called,repayment,time,paperwork,stating,rep,year,college</t>
+  </si>
+  <si>
+    <t>account,payment,customer,credit,service,check,called,sent,received,information,told,representative,bank,letter,issue,report,back,could,day,delinquent</t>
+  </si>
+  <si>
+    <t>call,phone,day,told,time,said,called,number,calling,asked,payment,even,back,know,one,never,person,got,stop,someone</t>
   </si>
 </sst>
 </file>
@@ -423,10 +423,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-0.08273896198486635</v>
+        <v>-0.0708726054971081</v>
       </c>
       <c r="B2">
-        <v>0.09618320610687023</v>
+        <v>0.09541984732824428</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>0.1441260582002455</v>
+        <v>0.1400158327575333</v>
       </c>
       <c r="B3">
         <v>0.3435114503816794</v>
@@ -451,10 +451,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-0.01336861211180364</v>
+        <v>-0.01495059315321198</v>
       </c>
       <c r="B4">
-        <v>0.1198473282442748</v>
+        <v>0.1206106870229008</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -465,10 +465,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-0.3004969641707594</v>
+        <v>-0.3101741051898327</v>
       </c>
       <c r="B5">
-        <v>0.05267175572519084</v>
+        <v>0.05190839694656488</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -479,10 +479,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>-0.2243951080702463</v>
+        <v>-0.2200793847966849</v>
       </c>
       <c r="B6">
-        <v>0.1694656488549618</v>
+        <v>0.1679389312977099</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>0.4768735882382202</v>
+        <v>0.4761604127767897</v>
       </c>
       <c r="B7">
-        <v>0.2183206106870229</v>
+        <v>0.2206106870229008</v>
       </c>
       <c r="C7">
         <v>5</v>

</xml_diff>

<commit_message>
updates to lemmatizer for more accuracy
</commit_message>
<xml_diff>
--- a/latent dirichlet allocation topics.xlsx
+++ b/latent dirichlet allocation topics.xlsx
@@ -28,22 +28,22 @@
     <t>Terms</t>
   </si>
   <si>
-    <t>payment,late,month,account,fee,pay,time,due,bank,make,bill,paid,day,online,never,even,check,one,every,charge</t>
-  </si>
-  <si>
-    <t>pay,month,job,year,money,payment,time,work,make,credit,go,one,people,could,help,like,college,even,back,going</t>
-  </si>
-  <si>
-    <t>payment,interest,pay,amount,rate,year,month,paid,paying,balance,principal,time,made,monthly,one,making,applied,owe,make,money</t>
-  </si>
-  <si>
-    <t>forbearance,told,received,deferment,form,letter,month,said,could,application,back,sent,called,repayment,time,paperwork,stating,rep,year,college</t>
-  </si>
-  <si>
-    <t>account,payment,customer,credit,service,check,called,sent,received,information,told,representative,bank,letter,issue,report,back,could,day,delinquent</t>
-  </si>
-  <si>
-    <t>call,phone,day,told,time,said,called,number,calling,asked,payment,even,back,know,one,never,person,got,stop,someone</t>
+    <t>payment,account,pay,month,check,make,interest,late,fee,bank,amount,charge,due,apply,send,take,time,balance,go,principal</t>
+  </si>
+  <si>
+    <t>call,customer,service,number,speak,representative,phone,contact,information,give,account,issue,try,time,one,hold,supervisor,problem,person,someone</t>
+  </si>
+  <si>
+    <t>tell,forbearance,receive,call,say,request,day,send,could,form,time,deferment,letter,state,ask,rep,month,payment,back,process</t>
+  </si>
+  <si>
+    <t>credit,report,receive,send,account,letter,collection,agency,delinquent,state,contact,never,show,due,still,information,default,mail,issue,owe</t>
+  </si>
+  <si>
+    <t>call,tell,say,payment,pay,time,day,phone,make,go,ask,harass,month,try,send,even,back,money,one,know</t>
+  </si>
+  <si>
+    <t>pay,go,payment,year,make,month,take,job,work,time,interest,money,college,one,could,help,tell,try,like,even</t>
   </si>
 </sst>
 </file>
@@ -423,10 +423,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-0.0708726054971081</v>
+        <v>-0.3288207330953067</v>
       </c>
       <c r="B2">
-        <v>0.09541984732824428</v>
+        <v>0.1694656488549618</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>0.1400158327575333</v>
+        <v>-0.006713715523267633</v>
       </c>
       <c r="B3">
-        <v>0.3435114503816794</v>
+        <v>0.07404580152671755</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -451,10 +451,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-0.01495059315321198</v>
+        <v>0.05709548479904948</v>
       </c>
       <c r="B4">
-        <v>0.1206106870229008</v>
+        <v>0.07404580152671755</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -465,10 +465,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-0.3101741051898327</v>
+        <v>-0.299271170347498</v>
       </c>
       <c r="B5">
-        <v>0.05190839694656488</v>
+        <v>0.04274809160305344</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -479,10 +479,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>-0.2200793847966849</v>
+        <v>0.4442888386644782</v>
       </c>
       <c r="B6">
-        <v>0.1679389312977099</v>
+        <v>0.2572519083969466</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>0.4761604127767897</v>
+        <v>0.1334213425059525</v>
       </c>
       <c r="B7">
-        <v>0.2206106870229008</v>
+        <v>0.3824427480916031</v>
       </c>
       <c r="C7">
         <v>5</v>

</xml_diff>